<commit_message>
previsões Mar-Mai + att grafico cesta
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Dropbox\PythonNotebooks\previsao_cestas\datasets_cestas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Dropbox\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AA3EDC-D2B8-45EF-9833-14EA25A6055F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB77C363-F794-4343-94FC-77639A91BCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -42,6 +42,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,11 +70,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -290,7 +297,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="B219" sqref="B219"/>
+      <selection activeCell="B220" sqref="B220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2043,12 +2050,16 @@
       </c>
     </row>
     <row r="219" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A219" s="3"/>
-      <c r="B219" s="1"/>
-    </row>
-    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="3">
+        <v>44958</v>
+      </c>
+      <c r="B219" s="1">
+        <v>572.92999999999995</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3"/>
-      <c r="B220" s="1"/>
+      <c r="B220" s="4"/>
     </row>
     <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="3"/>
@@ -2982,5 +2993,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Previsão Mai-Jul + att readme
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Dropbox\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57700002-5C0C-4622-A9A9-B3712C3A9086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFE3A36-0C7B-45CE-934D-86A842DBBF74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,8 +296,8 @@
   </sheetPr>
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="A221" sqref="A221"/>
+    <sheetView tabSelected="1" topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="B222" sqref="B222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2066,8 +2066,12 @@
       </c>
     </row>
     <row r="221" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A221" s="3"/>
-      <c r="B221" s="1"/>
+      <c r="A221" s="3">
+        <v>45017</v>
+      </c>
+      <c r="B221" s="1">
+        <v>547.54999999999995</v>
+      </c>
     </row>
     <row r="222" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="3"/>

</xml_diff>

<commit_message>
feat: previsão Jan-Mar 2024 + previsão completa 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DC7E08-EB6A-4ED2-B999-18CFCE9DE608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DD5458-CEB9-46E0-BC3B-0041AF20C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="E225" sqref="E225"/>
+      <selection activeCell="B230" sqref="B230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,8 +2259,12 @@
       </c>
     </row>
     <row r="229" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="5"/>
-      <c r="B229" s="3"/>
+      <c r="A229" s="5">
+        <v>45261</v>
+      </c>
+      <c r="B229" s="3">
+        <v>545.78</v>
+      </c>
     </row>
     <row r="230" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="5"/>

</xml_diff>

<commit_message>
feat: prev fev-abr 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DD5458-CEB9-46E0-BC3B-0041AF20C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF1F9B-F2C2-4099-AB90-46829A564EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="2355" windowWidth="16200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accb_custo_total_ilheus" sheetId="1" r:id="rId1"/>
@@ -424,8 +424,8 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
-      <selection activeCell="B230" sqref="B230"/>
+    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
+      <selection activeCell="B231" sqref="B231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,8 +2267,12 @@
       </c>
     </row>
     <row r="230" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="5"/>
-      <c r="B230" s="3"/>
+      <c r="A230" s="5">
+        <v>45292</v>
+      </c>
+      <c r="B230" s="3">
+        <v>547.63</v>
+      </c>
     </row>
     <row r="231" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="5"/>

</xml_diff>

<commit_message>
feat: prev mar-mai 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EF1F9B-F2C2-4099-AB90-46829A564EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5749DE46-D2DB-4560-943E-429BC0A61890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2355" windowWidth="16200" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accb_custo_total_ilheus" sheetId="1" r:id="rId1"/>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="B231" sqref="B231"/>
+      <selection activeCell="B232" sqref="B232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,8 +2275,12 @@
       </c>
     </row>
     <row r="231" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="5"/>
-      <c r="B231" s="3"/>
+      <c r="A231" s="5">
+        <v>45323</v>
+      </c>
+      <c r="B231" s="3">
+        <v>576.17999999999995</v>
+      </c>
     </row>
     <row r="232" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="5"/>

</xml_diff>

<commit_message>
feat: prev abr-jun 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5749DE46-D2DB-4560-943E-429BC0A61890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE46EAED-9358-4CA0-8D74-0FB60678741A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2283,8 +2283,12 @@
       </c>
     </row>
     <row r="232" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="5"/>
-      <c r="B232" s="3"/>
+      <c r="A232" s="5">
+        <v>45352</v>
+      </c>
+      <c r="B232" s="3">
+        <v>569.79</v>
+      </c>
     </row>
     <row r="233" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="5"/>

</xml_diff>

<commit_message>
feat: prev jul-set 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5206EBA3-30AB-40A0-A4DF-B0E1FF51178D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A811D073-9F77-4C6F-B983-C06E4D590D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,8 +424,8 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="B234" sqref="B234"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="B236" sqref="B236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2307,8 +2307,12 @@
       </c>
     </row>
     <row r="235" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="5"/>
-      <c r="B235" s="3"/>
+      <c r="A235" s="5">
+        <v>45444</v>
+      </c>
+      <c r="B235" s="3">
+        <v>563.89</v>
+      </c>
     </row>
     <row r="236" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="5"/>

</xml_diff>

<commit_message>
feat: prev ago-set 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A811D073-9F77-4C6F-B983-C06E4D590D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6CFD1C-8AB1-4D70-8472-E06CD4613A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B236" sqref="B236"/>
+      <selection activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,8 +2315,12 @@
       </c>
     </row>
     <row r="236" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="5"/>
-      <c r="B236" s="3"/>
+      <c r="A236" s="5">
+        <v>45474</v>
+      </c>
+      <c r="B236" s="3">
+        <v>510.14</v>
+      </c>
     </row>
     <row r="237" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="5"/>

</xml_diff>

<commit_message>
feat: prev set-nov 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\PythonNotebooks\previsao_cestas\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6CFD1C-8AB1-4D70-8472-E06CD4613A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC0FC22-51A0-4246-B11F-784C4DF1F16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B237" sqref="B237"/>
+      <selection activeCell="B238" sqref="B238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,8 +2323,12 @@
       </c>
     </row>
     <row r="237" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="5"/>
-      <c r="B237" s="3"/>
+      <c r="A237" s="5">
+        <v>45505</v>
+      </c>
+      <c r="B237" s="3">
+        <v>527.49</v>
+      </c>
       <c r="I237" s="9"/>
     </row>
     <row r="238" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: prev out-dez 2024
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC0FC22-51A0-4246-B11F-784C4DF1F16F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6CC2DD-5A4F-49EB-9820-3139CE420F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B238" sqref="B238"/>
+      <selection activeCell="B239" sqref="B239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2332,8 +2332,12 @@
       <c r="I237" s="9"/>
     </row>
     <row r="238" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="5"/>
-      <c r="B238" s="3"/>
+      <c r="A238" s="5">
+        <v>45536</v>
+      </c>
+      <c r="B238" s="3">
+        <v>531.09</v>
+      </c>
     </row>
     <row r="239" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="5"/>

</xml_diff>

<commit_message>
feat: add prev nov-jan 2024-2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E6CC2DD-5A4F-49EB-9820-3139CE420F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA0C1FC-9E8C-40F4-BCB7-12FADF2EB693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+      <selection activeCell="B240" sqref="B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2340,8 +2340,12 @@
       </c>
     </row>
     <row r="239" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="5"/>
-      <c r="B239" s="3"/>
+      <c r="A239" s="5">
+        <v>45566</v>
+      </c>
+      <c r="B239" s="3">
+        <v>543.77</v>
+      </c>
     </row>
     <row r="240" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="5"/>

</xml_diff>

<commit_message>
feat: prev dez-fev 2024-2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA0C1FC-9E8C-40F4-BCB7-12FADF2EB693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AA1900-A240-4FFD-B274-231D7E060864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B240" sqref="B240"/>
+      <selection activeCell="B241" sqref="B241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,8 +2348,12 @@
       </c>
     </row>
     <row r="240" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A240" s="5"/>
-      <c r="B240" s="3"/>
+      <c r="A240" s="5">
+        <v>45597</v>
+      </c>
+      <c r="B240" s="3">
+        <v>571.22</v>
+      </c>
     </row>
     <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="5"/>

</xml_diff>

<commit_message>
feat: prev fev-abr 2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93544ECF-1053-47D6-B163-0B51273057F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBCA71A-7302-42E3-946A-E4D7B75EFA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+      <selection activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2364,8 +2364,12 @@
       </c>
     </row>
     <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A242" s="5"/>
-      <c r="B242" s="3"/>
+      <c r="A242" s="5">
+        <v>45627</v>
+      </c>
+      <c r="B242" s="3">
+        <v>595.14</v>
+      </c>
     </row>
     <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="5"/>

</xml_diff>

<commit_message>
feat: prev mar-mai 2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBCA71A-7302-42E3-946A-E4D7B75EFA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E380863-91B0-43FE-B1AD-53A2648F4A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B243" sqref="B243"/>
+      <selection activeCell="B244" sqref="B244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2365,15 +2365,19 @@
     </row>
     <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="5">
-        <v>45627</v>
+        <v>45658</v>
       </c>
       <c r="B242" s="3">
         <v>595.14</v>
       </c>
     </row>
     <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A243" s="5"/>
-      <c r="B243" s="3"/>
+      <c r="A243" s="5">
+        <v>45689</v>
+      </c>
+      <c r="B243" s="3">
+        <v>607.77</v>
+      </c>
     </row>
     <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="5"/>

</xml_diff>

<commit_message>
feat: prev abr-jun 2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E380863-91B0-43FE-B1AD-53A2648F4A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1C21C1-C0AB-4A7A-B95C-1E978A25D7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accb_custo_total_ilheus" sheetId="1" r:id="rId1"/>
@@ -425,7 +425,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B244" sqref="B244"/>
+      <selection activeCell="B245" sqref="B245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,8 +2380,12 @@
       </c>
     </row>
     <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A244" s="5"/>
-      <c r="B244" s="3"/>
+      <c r="A244" s="5">
+        <v>45717</v>
+      </c>
+      <c r="B244" s="3">
+        <v>579.19000000000005</v>
+      </c>
     </row>
     <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="5"/>

</xml_diff>

<commit_message>
feat: prev mai-jun 2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1C21C1-C0AB-4A7A-B95C-1E978A25D7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1284A502-5159-4467-A24F-39A691BF70B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +66,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -94,7 +101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -117,6 +124,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +432,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
-      <selection activeCell="B245" sqref="B245"/>
+      <selection activeCell="N241" activeCellId="1" sqref="B246 N241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,15 +2365,16 @@
         <v>571.22</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="5">
         <v>45627</v>
       </c>
       <c r="B241" s="3">
         <v>583.49</v>
       </c>
-    </row>
-    <row r="242" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N241" s="9"/>
+    </row>
+    <row r="242" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="5">
         <v>45658</v>
       </c>
@@ -2371,7 +2382,7 @@
         <v>595.14</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="5">
         <v>45689</v>
       </c>
@@ -2379,7 +2390,7 @@
         <v>607.77</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="5">
         <v>45717</v>
       </c>
@@ -2387,51 +2398,55 @@
         <v>579.19000000000005</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A245" s="5"/>
-      <c r="B245" s="3"/>
-    </row>
-    <row r="246" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="5">
+        <v>45748</v>
+      </c>
+      <c r="B245" s="3">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="246" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="5"/>
-      <c r="B246" s="3"/>
-    </row>
-    <row r="247" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B246" s="10"/>
+    </row>
+    <row r="247" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="5"/>
       <c r="B247" s="3"/>
     </row>
-    <row r="248" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="5"/>
       <c r="B248" s="3"/>
     </row>
-    <row r="249" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="5"/>
       <c r="B249" s="3"/>
     </row>
-    <row r="250" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="5"/>
       <c r="B250" s="3"/>
     </row>
-    <row r="251" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="5"/>
       <c r="B251" s="3"/>
     </row>
-    <row r="252" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="5"/>
       <c r="B252" s="3"/>
     </row>
-    <row r="253" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="5"/>
       <c r="B253" s="3"/>
     </row>
-    <row r="254" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="5"/>
       <c r="B254" s="3"/>
     </row>
-    <row r="255" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="5"/>
       <c r="B255" s="3"/>
     </row>
-    <row r="256" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="5"/>
       <c r="B256" s="3"/>
     </row>

</xml_diff>

<commit_message>
feat: prev ago-out 2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15DB3108-9892-4D6A-A65E-D3BFF8BCB94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348BC31E-AFA4-43F0-9384-B6AF21443D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -309,13 +309,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A228" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E250" sqref="E250"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A241" sqref="A241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2300,8 +2300,12 @@
       </c>
     </row>
     <row r="248" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A248" s="7"/>
-      <c r="B248" s="5"/>
+      <c r="A248" s="7">
+        <v>45839</v>
+      </c>
+      <c r="B248" s="5">
+        <v>603.54999999999995</v>
+      </c>
       <c r="E248" s="10"/>
     </row>
     <row r="249" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat: add prev set-nov 2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348BC31E-AFA4-43F0-9384-B6AF21443D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B152C71-B9F5-43A5-86A3-D3890A3F2CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -310,7 +313,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A241" sqref="A241"/>
+      <selection activeCell="B250" sqref="B250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2309,8 +2312,12 @@
       <c r="E248" s="10"/>
     </row>
     <row r="249" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A249" s="7"/>
-      <c r="B249" s="5"/>
+      <c r="A249" s="7">
+        <v>45870</v>
+      </c>
+      <c r="B249" s="5">
+        <v>591.87</v>
+      </c>
     </row>
     <row r="250" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="7"/>

</xml_diff>

<commit_message>
feat: add prev out-dez 2025
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B152C71-B9F5-43A5-86A3-D3890A3F2CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E5EB6-22A3-49CC-A3A6-65717392CBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,7 +313,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B250" sqref="B250"/>
+      <selection activeCell="B251" sqref="B251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2320,8 +2320,12 @@
       </c>
     </row>
     <row r="250" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A250" s="7"/>
-      <c r="B250" s="5"/>
+      <c r="A250" s="7">
+        <v>45901</v>
+      </c>
+      <c r="B250" s="5">
+        <v>566.32000000000005</v>
+      </c>
     </row>
     <row r="251" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="7"/>

</xml_diff>

<commit_message>
feat: add prev nov-jan 2025-2026
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007E5EB6-22A3-49CC-A3A6-65717392CBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F1FCB0-3342-4A97-A4D6-77D31C15E4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,8 +312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B251" sqref="B251"/>
+    <sheetView tabSelected="1" topLeftCell="A243" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B252" sqref="B252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2328,8 +2328,12 @@
       </c>
     </row>
     <row r="251" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A251" s="7"/>
-      <c r="B251" s="5"/>
+      <c r="A251" s="7">
+        <v>45931</v>
+      </c>
+      <c r="B251" s="5">
+        <v>553.94000000000005</v>
+      </c>
     </row>
     <row r="252" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="7"/>

</xml_diff>

<commit_message>
feat: add prev dez-fev 2026
</commit_message>
<xml_diff>
--- a/data/accb_custo_total_ilheus.xlsx
+++ b/data/accb_custo_total_ilheus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\Documents\Meus Codes\previsao_cestas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F1FCB0-3342-4A97-A4D6-77D31C15E4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5ED6EFD-CB1F-4C44-9645-03EA64F9BA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,7 +313,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A243" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B252" sqref="B252"/>
+      <selection activeCell="B253" sqref="B253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2336,8 +2336,12 @@
       </c>
     </row>
     <row r="252" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A252" s="7"/>
-      <c r="B252" s="5"/>
+      <c r="A252" s="7">
+        <v>45962</v>
+      </c>
+      <c r="B252" s="5">
+        <v>451.39</v>
+      </c>
     </row>
     <row r="253" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="7"/>

</xml_diff>